<commit_message>
"Solver may change input data" bug fixed
</commit_message>
<xml_diff>
--- a/Task #1/Results.xlsx
+++ b/Task #1/Results.xlsx
@@ -448,11 +448,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="173282048"/>
-        <c:axId val="173283584"/>
+        <c:axId val="151331584"/>
+        <c:axId val="151333120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173282048"/>
+        <c:axId val="151331584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -462,15 +462,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173283584"/>
+        <c:crossAx val="151333120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="5"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173283584"/>
+        <c:axId val="151333120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -481,9 +482,9 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173282048"/>
+        <c:crossAx val="151331584"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -837,7 +838,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="B1" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -875,192 +876,263 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
       <c r="B2" t="n">
-        <v>-0.7334078501979615</v>
+        <v>-0.35046515366367464</v>
       </c>
       <c r="C2" t="n">
         <v>-5.0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.017728766960431526</v>
+        <v>0.17609125905568124</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.9030899869919435</v>
+        <v>0.17609125905568124</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.2041199826559248</v>
+        <v>0.17609125905568124</v>
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
       <c r="B3" t="n">
         <v>-5.0</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.3949344985323122</v>
+        <v>-0.12493873660829995</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.9030899869919435</v>
+        <v>-0.42596873227228116</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3010299956639812</v>
+        <v>-0.42596873227228116</v>
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
       <c r="B4" t="n">
         <v>-5.0</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.9365137424788943</v>
+        <v>-0.42596873227228116</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.9030899869919435</v>
+        <v>-1.0280287236002434</v>
       </c>
       <c r="F4" t="n">
+        <v>-1.0280287236002434</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-5.0</v>
+      </c>
+      <c r="D5" t="n">
         <v>-0.7269987279362623</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="n">
-        <v>-5.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-1.3491770079716363</v>
+      <c r="E5" t="n">
+        <v>-1.630088714928206</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.18293068358598671</v>
+        <v>-1.630088714928206</v>
       </c>
     </row>
     <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
       <c r="B6" t="n">
         <v>-5.0</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.8907562519182224</v>
+        <v>-1.0280287236002434</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-2.2321487062561682</v>
       </c>
       <c r="F6" t="n">
+        <v>-2.2321487062561682</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D7" t="n">
         <v>-1.3290587192642247</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="D7" t="n">
-        <v>-2.303419517410961</v>
+      <c r="E7" t="n">
+        <v>-2.8342086975841307</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.7849906749139491</v>
+        <v>-2.8342086975841307</v>
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
       <c r="D8" t="n">
-        <v>-2.844998761357585</v>
+        <v>-1.630088714928206</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-3.4362686889120932</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.9768762011528622</v>
+        <v>-3.4362686889120932</v>
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
       <c r="D9" t="n">
-        <v>-3.257662026850247</v>
+        <v>-1.9311187105921872</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-4.038328680240055</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.8704208702385754</v>
+        <v>-4.038328680240055</v>
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
       <c r="D10" t="n">
-        <v>-3.799241270797247</v>
+        <v>-2.2321487062561682</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-4.640388671568018</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.920394845200414</v>
+        <v>-4.640388671568018</v>
       </c>
     </row>
     <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
       <c r="D11" t="n">
-        <v>-4.211904536288525</v>
+        <v>-2.5331787019201495</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-5.0</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.8946894449655122</v>
+        <v>-5.0</v>
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
       <c r="D12" t="n">
-        <v>-4.753483780240824</v>
+        <v>-2.8342086975841307</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-5.0</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.9073519886344383</v>
+        <v>-5.0</v>
       </c>
     </row>
     <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
       <c r="D13" t="n">
-        <v>-5.0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>-0.9009745688693226</v>
+        <v>-3.135238693248112</v>
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
       <c r="D14" t="n">
-        <v>-5.0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-0.9041515726632892</v>
+        <v>-3.4362686889120932</v>
       </c>
     </row>
     <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
       <c r="D15" t="n">
-        <v>-5.0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>-0.9025601656722332</v>
+        <v>-3.7372986845760745</v>
       </c>
     </row>
     <row r="16">
-      <c r="F16" t="n">
-        <v>-0.9033551402341402</v>
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-4.038328680240055</v>
       </c>
     </row>
     <row r="17">
-      <c r="F17" t="n">
-        <v>-0.9029574710534354</v>
+      <c r="A17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-4.339358675904037</v>
       </c>
     </row>
     <row r="18">
-      <c r="F18" t="n">
-        <v>-0.9031562601272148</v>
+      <c r="A18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-4.640388671568018</v>
       </c>
     </row>
     <row r="19">
-      <c r="F19" t="n">
-        <v>-0.9030568542163907</v>
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-4.941418667231999</v>
       </c>
     </row>
     <row r="20">
-      <c r="F20" t="n">
-        <v>-0.9031065543276684</v>
+      <c r="A20" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-5.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="F21" t="n">
-        <v>-0.9030817035610773</v>
+      <c r="A21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-5.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="F22" t="n">
-        <v>-0.9030941287666246</v>
+      <c r="A22" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-5.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="F23" t="n">
-        <v>-0.9030879161194152</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="F24" t="n">
-        <v>-0.9030910224319108</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="F25" t="n">
-        <v>-0.9030894692728857</v>
+      <c r="A23" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-5.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>